<commit_message>
version 0.1 - main parameters are saved ok
</commit_message>
<xml_diff>
--- a/input/params_taggers.xlsx
+++ b/input/params_taggers.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="60" yWindow="5235" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$1</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -27,119 +26,101 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="28">
   <si>
-    <t xml:space="preserve">emi_master</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emi_parent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emi_sub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parameter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">task</t>
-  </si>
-  <si>
-    <t xml:space="preserve">area</t>
-  </si>
-  <si>
-    <t xml:space="preserve">family</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMI_0301</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMI_1005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMI_1039</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PP_CM_IPT_H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1st FD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AD-4833</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IPTs: 50%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IPTs: 90%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TILE_CM_THICKN_RESULT_MIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TILE_CM_THICKN_RESULT_MAX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMI_0801</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMI_1033</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1st TIC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SYR-322</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMI_1007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weight/Thickness/Hardness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coating</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMI_0401</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EMI_1066</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAK-491</t>
+    <t>emi_master</t>
+  </si>
+  <si>
+    <t>emi_parent</t>
+  </si>
+  <si>
+    <t>emi_sub</t>
+  </si>
+  <si>
+    <t>parameter</t>
+  </si>
+  <si>
+    <t>task</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>family</t>
+  </si>
+  <si>
+    <t>EMI_0301</t>
+  </si>
+  <si>
+    <t>EMI_1005</t>
+  </si>
+  <si>
+    <t>EMI_1039</t>
+  </si>
+  <si>
+    <t>PP_CM_IPT_H</t>
+  </si>
+  <si>
+    <t>1st FD</t>
+  </si>
+  <si>
+    <t>Compression</t>
+  </si>
+  <si>
+    <t>AD-4833</t>
+  </si>
+  <si>
+    <t>IPTs: 50%</t>
+  </si>
+  <si>
+    <t>IPTs: 90%</t>
+  </si>
+  <si>
+    <t>TILE_CM_THICKN_RESULT_MIN</t>
+  </si>
+  <si>
+    <t>TILE_CM_THICKN_RESULT_MAX</t>
+  </si>
+  <si>
+    <t>EMI_0801</t>
+  </si>
+  <si>
+    <t>EMI_1033</t>
+  </si>
+  <si>
+    <t>1st TIC</t>
+  </si>
+  <si>
+    <t>SYR-322</t>
+  </si>
+  <si>
+    <t>EMI_1007</t>
+  </si>
+  <si>
+    <t>Weight/Thickness/Hardness</t>
+  </si>
+  <si>
+    <t>Coating</t>
+  </si>
+  <si>
+    <t>EMI_0401</t>
+  </si>
+  <si>
+    <t>EMI_1066</t>
+  </si>
+  <si>
+    <t>TAK-491</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -157,7 +138,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -165,61 +146,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -278,38 +227,329 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="33.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="34.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="2" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="36.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.53"/>
+    <col min="1" max="2" width="15.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="1" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.42578125" style="1" customWidth="1"/>
+    <col min="6" max="7" width="15.28515625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="36.5703125" customWidth="1"/>
+    <col min="9" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -332,7 +572,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -355,7 +595,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -378,7 +618,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -401,7 +641,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -424,7 +664,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -447,7 +687,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -470,7 +710,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -493,7 +733,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -516,7 +756,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -539,7 +779,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -562,7 +802,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -585,7 +825,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -608,7 +848,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -631,7 +871,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
@@ -654,7 +894,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -677,7 +917,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
@@ -702,65 +942,39 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:G1"/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
+    <col min="1" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
+    <col min="1" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>